<commit_message>
Final ahora si :anguished:
</commit_message>
<xml_diff>
--- a/Excel/baseDatosPersonas.xlsx
+++ b/Excel/baseDatosPersonas.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Nombre</t>
   </si>
@@ -70,6 +70,15 @@
   </si>
   <si>
     <t>San José,Heredia,Cartago</t>
+  </si>
+  <si>
+    <t>Felipene Obando</t>
+  </si>
+  <si>
+    <t>felipeobando2001@gmail.com</t>
+  </si>
+  <si>
+    <t>San José,Alajuela,Heredia,Puntarenas,Guanacaste,Cartago,Limón</t>
   </si>
 </sst>
 </file>
@@ -422,7 +431,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8517FC3-2E04-4D5E-A355-59C59A745290}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:D2"/>
@@ -430,10 +439,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="17.5" collapsed="false"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="21.625" collapsed="false"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.0" collapsed="false"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="18.25" collapsed="false"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="21.625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="18.25" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -478,6 +487,20 @@
         <v>11</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>